<commit_message>
moved all files to correct region
</commit_message>
<xml_diff>
--- a/ALS-CLC 2024 as of May 2025.xlsx
+++ b/ALS-CLC 2024 as of May 2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29022"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimmy\OneDrive - Department of Education\b. PMU FILES\MONTHLY STATUS REPORT\2025\MAY 2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Work - Lawrence\Documents\DepEd_scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{EDE0DC33-1672-4E1E-B929-4661B2441122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5CC9E83-CBAA-4C5E-99C2-162C14DD2351}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205E17BF-8A6B-4A82-9501-84018C2F01C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B7017145-C2FD-4CA4-9487-5643B5A35313}"/>
+    <workbookView xWindow="-28920" yWindow="-5685" windowWidth="29040" windowHeight="15720" xr2:uid="{B7017145-C2FD-4CA4-9487-5643B5A35313}"/>
   </bookViews>
   <sheets>
     <sheet name="ALS-CLC 2024" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
     <definedName name="_EDU2">[2]EDU4!$G$10</definedName>
     <definedName name="_Fill" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="_Fill" hidden="1">#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALS-CLC 2024'!$A$6:$AI$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALS-CLC 2024'!$A$1:$AI$1</definedName>
     <definedName name="_Key1" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="_Key1" hidden="1">#REF!</definedName>
     <definedName name="_Key2" localSheetId="0" hidden="1">#REF!</definedName>
@@ -270,13 +270,13 @@
     <definedName name="ppmp2">#REF!</definedName>
     <definedName name="Prin" localSheetId="0">#REF!</definedName>
     <definedName name="Prin">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'ALS-CLC 2024'!$A$1:$I$10</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'ALS-CLC 2024'!$A$1:$I$5</definedName>
     <definedName name="_xlnm.Print_Area">#REF!</definedName>
     <definedName name="PRINT_AREA_MI" localSheetId="0">#REF!</definedName>
     <definedName name="PRINT_AREA_MI">#REF!</definedName>
     <definedName name="print_area_Mil" localSheetId="0">#REF!</definedName>
     <definedName name="print_area_Mil">#REF!</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'ALS-CLC 2024'!$2:$6</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'ALS-CLC 2024'!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles">#REF!</definedName>
     <definedName name="Print_Titles_MI" localSheetId="0">'[15]Enrolees&amp;Graduated'!$A$1:$IV$6,'[15]Enrolees&amp;Graduated'!$A$1:$A$65536</definedName>
     <definedName name="Print_Titles_MI">'[16]Enrolees&amp;Graduated'!$A$1:$IV$6,'[16]Enrolees&amp;Graduated'!$A$1:$A$65536</definedName>
@@ -416,19 +416,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="101">
-  <si>
-    <t>REPUBLIC OF THE PHILIPPINES</t>
-  </si>
-  <si>
-    <t>DEPARTMENT OF EDUCATION</t>
-  </si>
-  <si>
-    <t>CY 2024 ALS-CLCs</t>
-  </si>
-  <si>
-    <t>as of May 2025</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="97">
   <si>
     <t>Region</t>
   </si>
@@ -733,7 +721,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -758,22 +746,7 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -886,69 +859,53 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="2" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="2" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="5" fillId="3" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="3" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="3" borderId="3" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -958,11 +915,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -6922,9 +6874,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -6962,7 +6914,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -7068,7 +7020,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7210,7 +7162,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -7221,719 +7173,567 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:AG10"/>
+  <dimension ref="A1:AG5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <pane xSplit="3" ySplit="6" topLeftCell="H9" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="L11" sqref="L11"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D18" sqref="D18:D19"/>
       <selection pane="bottomLeft" activeCell="D18" sqref="D18:D19"/>
-      <selection pane="topRight" activeCell="D18" sqref="D18:D19"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A1:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="29" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="35.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="32.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="29.42578125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="36" style="35" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" style="5" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" style="6" customWidth="1"/>
-    <col min="13" max="14" width="16.85546875" style="7" customWidth="1"/>
-    <col min="15" max="16" width="16.85546875" style="2" customWidth="1"/>
-    <col min="17" max="20" width="16.85546875" style="7" customWidth="1"/>
-    <col min="21" max="21" width="29.5703125" style="7" customWidth="1"/>
-    <col min="22" max="23" width="16.85546875" style="2" customWidth="1"/>
-    <col min="24" max="32" width="9.140625" style="2"/>
-    <col min="33" max="33" width="17.42578125" style="2" customWidth="1"/>
-    <col min="34" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="19.265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.86328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="35.265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.3984375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.73046875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.3984375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="29.3984375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="36" style="19" customWidth="1"/>
+    <col min="10" max="10" width="16.86328125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="16.86328125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.86328125" style="4" customWidth="1"/>
+    <col min="13" max="14" width="16.86328125" style="5" customWidth="1"/>
+    <col min="15" max="16" width="16.86328125" style="1" customWidth="1"/>
+    <col min="17" max="20" width="16.86328125" style="5" customWidth="1"/>
+    <col min="21" max="21" width="29.59765625" style="5" customWidth="1"/>
+    <col min="22" max="23" width="16.86328125" style="1" customWidth="1"/>
+    <col min="24" max="32" width="9.1328125" style="1"/>
+    <col min="33" max="33" width="17.3984375" style="1" customWidth="1"/>
+    <col min="34" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:33" s="16" customFormat="1" ht="60.6" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="40"/>
-      <c r="M1" s="41"/>
-      <c r="N1" s="41"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
-      <c r="S1" s="41"/>
-      <c r="T1" s="41"/>
-      <c r="U1" s="41"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37"/>
-      <c r="AC1" s="37"/>
-      <c r="AD1" s="37"/>
-      <c r="AE1" s="37"/>
-      <c r="AF1" s="37"/>
-      <c r="AG1" s="37"/>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="6" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:33">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:33" s="18" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="20">
+        <v>131508</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="21">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="10">
-        <v>56000000</v>
-      </c>
-      <c r="J2" s="39"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="41"/>
-      <c r="R2" s="41"/>
-      <c r="S2" s="41"/>
-      <c r="T2" s="41"/>
-      <c r="U2" s="41"/>
-      <c r="V2" s="37"/>
-      <c r="W2" s="37"/>
-      <c r="X2" s="37"/>
-      <c r="Y2" s="37"/>
-      <c r="Z2" s="37"/>
-      <c r="AA2" s="37"/>
-      <c r="AB2" s="37"/>
-      <c r="AC2" s="37"/>
-      <c r="AD2" s="37"/>
-      <c r="AE2" s="37"/>
-      <c r="AF2" s="37"/>
-      <c r="AG2" s="37"/>
+      <c r="H2" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="22">
+        <v>14141414.140000001</v>
+      </c>
+      <c r="J2" s="23">
+        <v>14070707.07</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" s="24">
+        <v>1</v>
+      </c>
+      <c r="M2" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="S2" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="T2" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="U2" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="V2" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="W2" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="X2" s="17">
+        <f>IF($K2="Reverted",G2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Y2" s="17">
+        <f>IF($K2="Not yet started",G2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z2" s="17">
+        <f>IF($K2="Under Procurement",G2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA2" s="17">
+        <f>IF($K2="Ongoing",G2,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AB2" s="17">
+        <f>IF($K2="Completed",G2,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AC2" s="24">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="26">
+        <f>L2-AC2</f>
+        <v>0</v>
+      </c>
+      <c r="AE2" s="20"/>
+      <c r="AF2" s="20">
+        <v>4.25</v>
+      </c>
+      <c r="AG2" s="20" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="3" spans="1:33">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="10">
-        <f>I2-I4</f>
+    <row r="3" spans="1:33" s="18" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="20">
+        <v>100684</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="21">
+        <v>1</v>
+      </c>
+      <c r="H3" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="I3" s="22">
+        <v>12871493.449999999</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3" s="24">
+        <v>0.8</v>
+      </c>
+      <c r="M3" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="25"/>
+      <c r="O3" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="P3" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q3" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="R3" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="S3" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="T3" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="U3" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="V3" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="W3" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="X3" s="17">
+        <f t="shared" ref="X3:X5" si="0">IF($K3="Reverted",G3,0)</f>
         <v>0</v>
       </c>
-      <c r="J3" s="39"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="41"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="41"/>
-      <c r="R3" s="41"/>
-      <c r="S3" s="41"/>
-      <c r="T3" s="41"/>
-      <c r="U3" s="41"/>
-      <c r="V3" s="37"/>
-      <c r="W3" s="37"/>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="37"/>
-      <c r="AB3" s="37"/>
-      <c r="AC3" s="37"/>
-      <c r="AD3" s="37"/>
-      <c r="AE3" s="37"/>
-      <c r="AF3" s="37"/>
-      <c r="AG3" s="37"/>
+      <c r="Y3" s="17">
+        <f t="shared" ref="Y3:Y5" si="1">IF($K3="Not yet started",G3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="Z3" s="17">
+        <f t="shared" ref="Z3:Z5" si="2">IF($K3="Under Procurement",G3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AA3" s="17">
+        <f t="shared" ref="AA3:AA5" si="3">IF($K3="Ongoing",G3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="AB3" s="17">
+        <f t="shared" ref="AB3:AB5" si="4">IF($K3="Completed",G3,0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC3" s="24">
+        <v>0.6</v>
+      </c>
+      <c r="AD3" s="26">
+        <f t="shared" ref="AD3:AD5" si="5">L3-AC3</f>
+        <v>0.20000000000000007</v>
+      </c>
+      <c r="AE3" s="20"/>
+      <c r="AF3" s="20"/>
+      <c r="AG3" s="20" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="4" spans="1:33" s="1" customFormat="1">
-      <c r="G4" s="11">
-        <f>SUBTOTAL(9,G7:G10)</f>
-        <v>4</v>
-      </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="10">
-        <f>SUBTOTAL(9,I7:I10)</f>
-        <v>56000000</v>
-      </c>
-      <c r="J4" s="13"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="15"/>
-    </row>
-    <row r="5" spans="1:33" s="16" customFormat="1">
-      <c r="A5" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="17"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="19"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-    </row>
-    <row r="6" spans="1:33" s="32" customFormat="1" ht="60.6" customHeight="1">
-      <c r="A6" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="L6" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="M6" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="N6" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="O6" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="P6" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q6" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="R6" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="S6" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="T6" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="U6" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="V6" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="W6" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="X6" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y6" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z6" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA6" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="AB6" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC6" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD6" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE6" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="AF6" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="AG6" s="22" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33" s="34" customFormat="1" ht="154.5" customHeight="1">
-      <c r="A7" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" s="36">
-        <v>131508</v>
-      </c>
-      <c r="D7" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="36" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="42">
+    <row r="4" spans="1:33" s="18" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" s="20">
+        <v>300690</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="21">
         <v>1</v>
       </c>
-      <c r="H7" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" s="43">
-        <v>14141414.140000001</v>
-      </c>
-      <c r="J7" s="44">
-        <v>14070707.07</v>
-      </c>
-      <c r="K7" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="L7" s="45">
-        <v>1</v>
-      </c>
-      <c r="M7" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="N7" s="46" t="s">
-        <v>45</v>
-      </c>
-      <c r="O7" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="P7" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q7" s="46" t="s">
-        <v>47</v>
-      </c>
-      <c r="R7" s="46" t="s">
-        <v>48</v>
-      </c>
-      <c r="S7" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="T7" s="46" t="s">
-        <v>50</v>
-      </c>
-      <c r="U7" s="46" t="s">
-        <v>51</v>
-      </c>
-      <c r="V7" s="36" t="s">
-        <v>52</v>
-      </c>
-      <c r="W7" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="X7" s="33">
-        <f>IF($K7="Reverted",G7,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Y7" s="33">
-        <f>IF($K7="Not yet started",G7,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z7" s="33">
-        <f>IF($K7="Under Procurement",G7,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AA7" s="33">
-        <f>IF($K7="Ongoing",G7,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AB7" s="33">
-        <f>IF($K7="Completed",G7,0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC7" s="45">
-        <v>1</v>
-      </c>
-      <c r="AD7" s="47">
-        <f>L7-AC7</f>
-        <v>0</v>
-      </c>
-      <c r="AE7" s="36"/>
-      <c r="AF7" s="36">
-        <v>4.25</v>
-      </c>
-      <c r="AG7" s="36" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:33" s="34" customFormat="1" ht="154.5" customHeight="1">
-      <c r="A8" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="36">
-        <v>100684</v>
-      </c>
-      <c r="D8" s="36" t="s">
+      <c r="H4" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" s="22">
+        <v>12446387.1</v>
+      </c>
+      <c r="J4" s="23">
+        <v>10458975.449999999</v>
+      </c>
+      <c r="K4" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="42">
-        <v>1</v>
-      </c>
-      <c r="H8" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="I8" s="43">
-        <v>12871493.449999999</v>
-      </c>
-      <c r="J8" s="44" t="s">
-        <v>60</v>
-      </c>
-      <c r="K8" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="L8" s="45">
-        <v>0.8</v>
-      </c>
-      <c r="M8" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="N8" s="46"/>
-      <c r="O8" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="P8" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q8" s="46" t="s">
-        <v>65</v>
-      </c>
-      <c r="R8" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="S8" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="T8" s="46" t="s">
-        <v>68</v>
-      </c>
-      <c r="U8" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="V8" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="W8" s="36" t="s">
-        <v>71</v>
-      </c>
-      <c r="X8" s="33">
-        <f t="shared" ref="X8:X10" si="0">IF($K8="Reverted",G8,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Y8" s="33">
-        <f t="shared" ref="Y8:Y10" si="1">IF($K8="Not yet started",G8,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z8" s="33">
-        <f t="shared" ref="Z8:Z10" si="2">IF($K8="Under Procurement",G8,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AA8" s="33">
-        <f t="shared" ref="AA8:AA10" si="3">IF($K8="Ongoing",G8,0)</f>
-        <v>1</v>
-      </c>
-      <c r="AB8" s="33">
-        <f t="shared" ref="AB8:AB10" si="4">IF($K8="Completed",G8,0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC8" s="45">
-        <v>0.6</v>
-      </c>
-      <c r="AD8" s="47">
-        <f t="shared" ref="AD8:AD10" si="5">L8-AC8</f>
-        <v>0.20000000000000007</v>
-      </c>
-      <c r="AE8" s="36"/>
-      <c r="AF8" s="36"/>
-      <c r="AG8" s="36" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:33" s="34" customFormat="1" ht="154.5" customHeight="1">
-      <c r="A9" s="36" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="36">
-        <v>300690</v>
-      </c>
-      <c r="D9" s="36" t="s">
+      <c r="L4" s="24">
+        <v>0.7</v>
+      </c>
+      <c r="M4" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="E9" s="36" t="s">
+      <c r="N4" s="25"/>
+      <c r="O4" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="F9" s="36" t="s">
+      <c r="P4" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="G9" s="42">
-        <v>1</v>
-      </c>
-      <c r="H9" s="36" t="s">
+      <c r="Q4" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="I9" s="43">
-        <v>12446387.1</v>
-      </c>
-      <c r="J9" s="44">
-        <v>10458975.449999999</v>
-      </c>
-      <c r="K9" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="L9" s="45">
-        <v>0.7</v>
-      </c>
-      <c r="M9" s="46" t="s">
+      <c r="R4" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="N9" s="46"/>
-      <c r="O9" s="36" t="s">
+      <c r="S4" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="P9" s="36" t="s">
+      <c r="T4" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="Q9" s="46" t="s">
+      <c r="U4" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="R9" s="46" t="s">
+      <c r="V4" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="S9" s="46" t="s">
+      <c r="W4" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="T9" s="46" t="s">
-        <v>84</v>
-      </c>
-      <c r="U9" s="46" t="s">
-        <v>85</v>
-      </c>
-      <c r="V9" s="36" t="s">
-        <v>86</v>
-      </c>
-      <c r="W9" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="X9" s="33">
+      <c r="X4" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Y9" s="33">
+      <c r="Y4" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Z9" s="33">
+      <c r="Z4" s="17">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA9" s="33">
+      <c r="AA4" s="17">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="AB9" s="33">
+      <c r="AB4" s="17">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AC9" s="45">
+      <c r="AC4" s="24">
         <v>0.5</v>
       </c>
-      <c r="AD9" s="47">
+      <c r="AD4" s="26">
         <f t="shared" si="5"/>
         <v>0.19999999999999996</v>
       </c>
-      <c r="AE9" s="36"/>
-      <c r="AF9" s="36"/>
-      <c r="AG9" s="36" t="s">
-        <v>41</v>
+      <c r="AE4" s="20"/>
+      <c r="AF4" s="20"/>
+      <c r="AG4" s="20" t="s">
+        <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:33" s="34" customFormat="1" ht="154.5" customHeight="1">
-      <c r="A10" s="36" t="s">
+    <row r="5" spans="1:33" s="18" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="20">
+        <v>301596</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="21">
+        <v>1</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="22">
+        <v>16540705.310000001</v>
+      </c>
+      <c r="J5" s="23">
+        <v>16458637.91</v>
+      </c>
+      <c r="K5" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" s="24">
+        <v>1</v>
+      </c>
+      <c r="M5" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="N5" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="C10" s="36">
-        <v>301596</v>
-      </c>
-      <c r="D10" s="36" t="s">
+      <c r="O5" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="E10" s="36" t="s">
+      <c r="P5" s="20"/>
+      <c r="Q5" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="F10" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="G10" s="42">
-        <v>1</v>
-      </c>
-      <c r="H10" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="I10" s="43">
-        <v>16540705.310000001</v>
-      </c>
-      <c r="J10" s="44">
-        <v>16458637.91</v>
-      </c>
-      <c r="K10" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="L10" s="45">
-        <v>1</v>
-      </c>
-      <c r="M10" s="46" t="s">
+      <c r="R5" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="N10" s="46" t="s">
+      <c r="S5" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="O10" s="36" t="s">
+      <c r="T5" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="U5" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="P10" s="36"/>
-      <c r="Q10" s="46" t="s">
+      <c r="V5" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="R10" s="46" t="s">
+      <c r="W5" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="S10" s="46" t="s">
-        <v>97</v>
-      </c>
-      <c r="T10" s="46" t="s">
-        <v>48</v>
-      </c>
-      <c r="U10" s="46" t="s">
-        <v>98</v>
-      </c>
-      <c r="V10" s="36" t="s">
-        <v>99</v>
-      </c>
-      <c r="W10" s="36" t="s">
-        <v>100</v>
-      </c>
-      <c r="X10" s="33">
+      <c r="X5" s="17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Y10" s="33">
+      <c r="Y5" s="17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Z10" s="33">
+      <c r="Z5" s="17">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA10" s="33">
+      <c r="AA5" s="17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AB10" s="33">
+      <c r="AB5" s="17">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="AC10" s="45">
+      <c r="AC5" s="24">
         <v>0.83</v>
       </c>
-      <c r="AD10" s="47">
+      <c r="AD5" s="26">
         <f t="shared" si="5"/>
         <v>0.17000000000000004</v>
       </c>
-      <c r="AE10" s="36"/>
-      <c r="AF10" s="36"/>
-      <c r="AG10" s="36" t="s">
-        <v>54</v>
+      <c r="AE5" s="20"/>
+      <c r="AF5" s="20"/>
+      <c r="AG5" s="20" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A6:AI10" xr:uid="{99C032EF-7820-46FF-8D85-6FD79A9510C8}"/>
-  <conditionalFormatting sqref="C8">
+  <autoFilter ref="A1:AI5" xr:uid="{99C032EF-7820-46FF-8D85-6FD79A9510C8}"/>
+  <conditionalFormatting sqref="C3">
     <cfRule type="duplicateValues" dxfId="4" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C10">
+  <conditionalFormatting sqref="C5">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11:C1048576 C2:C7 C9">
+  <conditionalFormatting sqref="C6:C1048576 C1:C2 C4">
     <cfRule type="duplicateValues" dxfId="2" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J7:W10">
+  <conditionalFormatting sqref="J2:W5">
     <cfRule type="containsBlanks" dxfId="1" priority="1">
-      <formula>LEN(TRIM(J7))=0</formula>
+      <formula>LEN(TRIM(J2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC7:AC10">
+  <conditionalFormatting sqref="AC2:AC5">
     <cfRule type="containsBlanks" dxfId="0" priority="2">
-      <formula>LEN(TRIM(AC7))=0</formula>
+      <formula>LEN(TRIM(AC2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>

</xml_diff>